<commit_message>
Changes made to algorithms
</commit_message>
<xml_diff>
--- a/g1.xlsx
+++ b/g1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elliot\Documents\Github\Uni_ASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1D3358-73F4-479B-AB8A-D2D721399938}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FA3831-A8D0-4AC5-8BA8-3A69D9228109}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18300" yWindow="3675" windowWidth="21600" windowHeight="12735" xr2:uid="{D44875D0-06F7-43A2-B0F9-916B25F2552A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D44875D0-06F7-43A2-B0F9-916B25F2552A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,6 +106,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>unordered_map</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> with list</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -262,6 +292,7 @@
         <c:axId val="1616366480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -449,6 +480,34 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>map with list</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -605,6 +664,7 @@
         <c:axId val="1547794640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -792,6 +852,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>map with list</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -948,6 +1038,7 @@
         <c:axId val="1710156704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1134,37 +1225,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1419,6 +1480,7 @@
         <c:axId val="1710103120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3887,15 +3949,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3959,15 +4021,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4294,8 +4356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42114FEC-1ADE-4E99-ABA6-E58775BDA7F5}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>